<commit_message>
Added in revisions 2.0
</commit_message>
<xml_diff>
--- a/TCEQ_Data.xlsx
+++ b/TCEQ_Data.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Cases" sheetId="1" r:id="rId1"/>
+    <sheet name="Incident Sums" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2046" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2065" uniqueCount="293">
   <si>
     <t>INCIDENT NO.</t>
   </si>
@@ -10100,4 +10101,197 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2">
+        <f>SUMIF(Cases!A:A,'Incident Sums'!A2,Cases!M:M)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3">
+        <f>SUMIF(Cases!A:A,'Incident Sums'!A3,Cases!M:M)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4">
+        <f>SUMIF(Cases!A:A,'Incident Sums'!A4,Cases!M:M)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5">
+        <f>SUMIF(Cases!A:A,'Incident Sums'!A5,Cases!M:M)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6">
+        <f>SUMIF(Cases!A:A,'Incident Sums'!A6,Cases!M:M)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7">
+        <f>SUMIF(Cases!A:A,'Incident Sums'!A7,Cases!M:M)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8">
+        <f>SUMIF(Cases!A:A,'Incident Sums'!A8,Cases!M:M)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B9">
+        <f>SUMIF(Cases!A:A,'Incident Sums'!A9,Cases!M:M)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B10">
+        <f>SUMIF(Cases!A:A,'Incident Sums'!A10,Cases!M:M)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B11">
+        <f>SUMIF(Cases!A:A,'Incident Sums'!A11,Cases!M:M)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B12">
+        <f>SUMIF(Cases!A:A,'Incident Sums'!A12,Cases!M:M)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B13">
+        <f>SUMIF(Cases!A:A,'Incident Sums'!A13,Cases!M:M)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B14">
+        <f>SUMIF(Cases!A:A,'Incident Sums'!A14,Cases!M:M)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B15">
+        <f>SUMIF(Cases!A:A,'Incident Sums'!A15,Cases!M:M)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B16">
+        <f>SUMIF(Cases!A:A,'Incident Sums'!A16,Cases!M:M)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B17">
+        <f>SUMIF(Cases!A:A,'Incident Sums'!A17,Cases!M:M)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B18">
+        <f>SUMIF(Cases!A:A,'Incident Sums'!A18,Cases!M:M)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="A9" r:id="rId8"/>
+    <hyperlink ref="A10" r:id="rId9"/>
+    <hyperlink ref="A11" r:id="rId10"/>
+    <hyperlink ref="A12" r:id="rId11"/>
+    <hyperlink ref="A13" r:id="rId12"/>
+    <hyperlink ref="A14" r:id="rId13"/>
+    <hyperlink ref="A15" r:id="rId14"/>
+    <hyperlink ref="A16" r:id="rId15"/>
+    <hyperlink ref="A17" r:id="rId16"/>
+    <hyperlink ref="A18" r:id="rId17"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>